<commit_message>
before parent iop was assigned using the top iop increased parent p pipe, but the exact parent iop need to be set, now rectified
</commit_message>
<xml_diff>
--- a/ft1.xlsx
+++ b/ft1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,342 +436,122 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 0</t>
+          <t>start_node</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>start_node</t>
+          <t>end_node</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>end_node</t>
+          <t>length</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>manual_iop</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>ground_level_start</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>ground_level_end</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>discharge</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>length</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>ground_level_start</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>ground_level_end</t>
-        </is>
-      </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>manual_iop</t>
+          <t>new_iop</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>new_iop</t>
+          <t>new_velocity</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>new_velocity</t>
+          <t>new_fhl</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>new_fhl</t>
+          <t>available_residual_head_at_start</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>available_residual_head_at_start</t>
+          <t>residual_head_at_end</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>residual_head_at_end</t>
+          <t>allowed_iops</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>allowed_iops</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>opti_count</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>209</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>DC</t>
+        </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>J-4105</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>J-4106</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>0.02155</v>
-      </c>
+          <t>J1</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>200</v>
+      </c>
+      <c r="D2" t="inlineStr"/>
       <c r="E2" t="n">
-        <v>191.67</v>
+        <v>70</v>
       </c>
       <c r="F2" t="n">
-        <v>191.34</v>
+        <v>50</v>
       </c>
       <c r="G2" t="n">
-        <v>188.32</v>
-      </c>
-      <c r="H2" t="inlineStr"/>
+        <v>4</v>
+      </c>
+      <c r="H2" t="n">
+        <v>2500</v>
+      </c>
       <c r="I2" t="n">
-        <v>142.8</v>
+        <v>0.82</v>
       </c>
       <c r="J2" t="n">
-        <v>1.35</v>
+        <v>0.033144</v>
       </c>
       <c r="K2" t="n">
-        <v>2.374578</v>
+        <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>41.037195</v>
-      </c>
-      <c r="M2" t="n">
-        <v>41.682617</v>
+        <v>19.966856</v>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>[1400, 1500, 1600, 1700, 1800, 1900, 2000, 2100, 2200, 2300, 2400, 2500]</t>
+        </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>[96.8, 111.6, 125, 142.8, 160.8, 178.6, 201]</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>['V33_C15', 'V33_C14']</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>461</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>J-3975</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>J-3976</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>0.01251</v>
-      </c>
-      <c r="E3" t="n">
-        <v>264.63</v>
-      </c>
-      <c r="F3" t="n">
-        <v>190.02</v>
-      </c>
-      <c r="G3" t="n">
-        <v>192.13</v>
-      </c>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="n">
-        <v>160.8</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0.62</v>
-      </c>
-      <c r="K3" t="n">
-        <v>0.692109</v>
-      </c>
-      <c r="L3" t="n">
-        <v>43.345283</v>
-      </c>
-      <c r="M3" t="n">
-        <v>40.543174</v>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>[96.8, 111.6, 125, 142.8, 160.8]</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>['V44_C1', 'V44_C1', 'V44_C1', 'V44_C1', 'V44_C1', 'V44_C1', 'V44_C1', 'V44_C1', 'V44_C1', 'V44_C1', 'V44_C1', 'V44_C12']</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>483</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>J-4099</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>J-4100</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>0.01352</v>
-      </c>
-      <c r="E4" t="n">
-        <v>305.14</v>
-      </c>
-      <c r="F4" t="n">
-        <v>188.33</v>
-      </c>
-      <c r="G4" t="n">
-        <v>184.4</v>
-      </c>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="n">
-        <v>160.8</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0.67</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0.918473</v>
-      </c>
-      <c r="L4" t="n">
-        <v>42.84711</v>
-      </c>
-      <c r="M4" t="n">
-        <v>45.858637</v>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>[96.8, 111.6, 125, 142.8, 160.8]</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>['V35_C25', 'V35_C25', 'V35_C26']</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>559</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>J-4195</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>J-4196</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>0.02235</v>
-      </c>
-      <c r="E5" t="n">
-        <v>172.14</v>
-      </c>
-      <c r="F5" t="n">
-        <v>158.26</v>
-      </c>
-      <c r="G5" t="n">
-        <v>158.75</v>
-      </c>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="n">
-        <v>201</v>
-      </c>
-      <c r="J5" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="K5" t="n">
-        <v>0.439984</v>
-      </c>
-      <c r="L5" t="n">
-        <v>30.108421</v>
-      </c>
-      <c r="M5" t="n">
-        <v>29.178437</v>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>[111.6, 125, 142.8, 160.8, 178.6, 201]</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>['V20_C22', 'V20_C22', 'V20_C22', 'V20_C22', 'V20_C12']</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>728</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>J-3897</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>J-3898</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>0.03088</v>
-      </c>
-      <c r="E6" t="n">
-        <v>413.34</v>
-      </c>
-      <c r="F6" t="n">
-        <v>179.06</v>
-      </c>
-      <c r="G6" t="n">
-        <v>183.09</v>
-      </c>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="n">
-        <v>160.8</v>
-      </c>
-      <c r="J6" t="n">
-        <v>1.52</v>
-      </c>
-      <c r="K6" t="n">
-        <v>5.547828</v>
-      </c>
-      <c r="L6" t="n">
-        <v>38.138721</v>
-      </c>
-      <c r="M6" t="n">
-        <v>28.560893</v>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>[125, 142.8, 160.8, 178.6, 201, 223.4, 250.4]</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>['V23_C10', 'V24_C7']</t>
+          <t>['V2', 'V1', 'V1', 'V1', 'V1', 'V1', 'V1', 'V1', 'V1', 'V1', 'V1']</t>
         </is>
       </c>
     </row>

</xml_diff>